<commit_message>
Topic colofon translated. Added screendumps and solutions files. Corrections to practice file Advertising campaign.
</commit_message>
<xml_diff>
--- a/practicefiles/Advertising_Campaign.xlsx
+++ b/practicefiles/Advertising_Campaign.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\office\excel2016en - oude-kopie\practicefiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="13440" windowHeight="12330"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="13440" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,51 +24,51 @@
     <definedName name="Zoeklijst">[1]harddisks!$B$11:$E$22</definedName>
     <definedName name="Zoeknr">[1]harddisks!$D$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Aantal verstuurd</t>
+    <t>Number of flyers sent</t>
   </si>
   <si>
-    <t>Respons (%)</t>
+    <t>Printing costs per piece</t>
   </si>
   <si>
-    <t>Drukkosten per stuk</t>
+    <t>Shipping costs per piece</t>
   </si>
   <si>
-    <t>Verzendkosten per stuk</t>
+    <t>Response (%)</t>
   </si>
   <si>
-    <t>Opbrengst per respons</t>
+    <t>Response (number)</t>
   </si>
   <si>
-    <t>Respons (aantal reacties)</t>
+    <t>Revenue per response</t>
   </si>
   <si>
-    <t>Opbrengst totaal</t>
+    <t>Revenue total</t>
   </si>
   <si>
-    <t>Kosten totaal</t>
+    <t>Costs total</t>
   </si>
   <si>
-    <t>Winst</t>
+    <t>profit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0;[Red]&quot;€&quot;\ \-#,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00;&quot;€&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ &quot;€&quot;\ * #,##0_ ;_ &quot;€&quot;\ * \-#,##0_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +84,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,10 +98,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -147,35 +159,39 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Standaard 2" xfId="2"/>
-    <cellStyle name="Valuta 2" xfId="3"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
+    <cellStyle name="Valuta 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -405,7 +421,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -447,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -480,9 +496,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -515,6 +548,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -690,17 +740,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="9" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="9.7109375" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -713,62 +763,62 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>2.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="5">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <f>B2*B1</f>
         <v>4500</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <f>B8*B6</f>
         <v>198000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <f>B1*(B4+B5)</f>
         <v>180000</v>
       </c>
@@ -777,145 +827,145 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="8">
         <f>B9-B10</f>
         <v>18000</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8">
+      <c r="B14" s="9">
         <f>B11</f>
         <v>18000</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="10">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="10">
         <v>0.02</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="10">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="10">
         <v>2.75E-2</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="10">
         <v>0.03</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="10">
+      <c r="B15" s="11">
         <v>100000</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="10">
+      <c r="B16" s="11">
         <v>125000</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="10">
+      <c r="B17" s="11">
         <v>150000</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="10">
+      <c r="B18" s="11">
         <v>175000</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="10">
+      <c r="B19" s="11">
         <v>200000</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="10">
+      <c r="B20" s="11">
         <v>225000</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="10">
+      <c r="B21" s="11">
         <v>250000</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="10">
+      <c r="B22" s="11">
         <v>275000</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="10">
+      <c r="B23" s="11">
         <v>300000</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>